<commit_message>
faster homepage. data update
</commit_message>
<xml_diff>
--- a/data/Workbook1.xlsx
+++ b/data/Workbook1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="334">
   <si>
     <t>headline</t>
   </si>
@@ -1057,6 +1057,36 @@
   </si>
   <si>
     <t>img/dwarka/comic.jpg</t>
+  </si>
+  <si>
+    <t>Farm Lands in the village of Madanur Khadar</t>
+  </si>
+  <si>
+    <t>The farmers in Madanpur Khadar owned the lands around the small village and used them to grow upto two crops of wheat and pulses</t>
+  </si>
+  <si>
+    <t>DDA Survey Conducted</t>
+  </si>
+  <si>
+    <t>Survey conducted by DDA for Slum Clearence in Bastis of Alaknanda, Nehru Place, Yusuf Sarai, Green Park</t>
+  </si>
+  <si>
+    <t>Petition Signed by Basti Residents</t>
+  </si>
+  <si>
+    <t>Petition signed by Alaknanda residents to remove the slums.</t>
+  </si>
+  <si>
+    <t>Eviction in Bastis</t>
+  </si>
+  <si>
+    <t>People were evicted from the bastis and promised plots in site near Apollo Hospital. The site then shifted to Madanpur Khadar .People mobilised to their allotted plots with their belongings</t>
+  </si>
+  <si>
+    <t>Madanpur Khadar Development Period</t>
+  </si>
+  <si>
+    <t>The society has evolved since 2002 with no facilities and amenities provided during rehabilitation process.</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1205,6 +1235,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1541,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1696,7 +1727,7 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1730,10 +1761,10 @@
       <c r="R2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="T2" s="25" t="s">
         <v>172</v>
       </c>
       <c r="U2" s="1">
@@ -1742,7 +1773,7 @@
       <c r="V2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="25" t="s">
         <v>174</v>
       </c>
       <c r="X2" s="1">
@@ -1751,7 +1782,7 @@
       <c r="Y2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="Z2" s="25" t="s">
         <v>176</v>
       </c>
       <c r="AA2" s="1">
@@ -1760,7 +1791,7 @@
       <c r="AB2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC2" s="25" t="s">
         <v>179</v>
       </c>
       <c r="AD2" s="1">
@@ -1769,7 +1800,7 @@
       <c r="AE2" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AF2" s="24" t="s">
+      <c r="AF2" s="25" t="s">
         <v>178</v>
       </c>
       <c r="AG2" s="1">
@@ -1780,22 +1811,22 @@
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1828,81 +1859,81 @@
       <c r="R3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="S3" s="25" t="s">
+      <c r="S3" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3" s="26">
         <v>1980</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="V3" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="W3" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="26">
         <v>1984</v>
       </c>
-      <c r="Y3" s="25" t="s">
+      <c r="Y3" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="Z3" s="25" t="s">
+      <c r="Z3" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="AA3" s="25">
+      <c r="AA3" s="26">
         <v>1990</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="AB3" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AC3" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="AD3" s="25">
+      <c r="AD3" s="26">
         <v>2009</v>
       </c>
-      <c r="AE3" s="25" t="s">
+      <c r="AE3" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="AF3" s="25" t="s">
+      <c r="AF3" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="AG3" s="25">
+      <c r="AG3" s="26">
         <v>2010</v>
       </c>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3"/>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="3"/>
-      <c r="AQ3" s="3"/>
-      <c r="AR3" s="3"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
     </row>
     <row r="4" spans="1:44" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1926,99 +1957,99 @@
       <c r="O4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="S4" s="25" t="s">
+      <c r="S4" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="26">
         <v>1985</v>
       </c>
-      <c r="V4" s="25" t="s">
+      <c r="V4" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="W4" s="25" t="s">
+      <c r="W4" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="X4" s="25">
+      <c r="X4" s="26">
         <v>2004</v>
       </c>
-      <c r="Y4" s="25" t="s">
+      <c r="Y4" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="AA4" s="25">
+      <c r="AA4" s="26">
         <v>2007</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AB4" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AC4" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="AD4" s="25">
+      <c r="AD4" s="26">
         <v>2008</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AE4" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AF4" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="AG4" s="25">
+      <c r="AG4" s="26">
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:44" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:44" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="S5" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="T5" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5" s="26">
         <v>2012</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="W5" s="25" t="s">
+      <c r="W5" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="26">
         <v>2016</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="Y5" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="Z5" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="AA5" s="25">
+      <c r="AA5" s="26">
         <v>2017</v>
       </c>
     </row>
@@ -2026,13 +2057,13 @@
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2041,7 +2072,7 @@
       <c r="F6" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2074,63 +2105,63 @@
       <c r="R6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="4">
         <v>1970</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="4">
         <v>2007</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AA6" s="4">
         <v>2015</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AD6" s="4">
         <v>2017</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AG6" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:44" ht="118" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2139,7 +2170,7 @@
       <c r="F7" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2172,196 +2203,244 @@
       <c r="R7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="S7" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="T7" s="25" t="s">
+      <c r="T7" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="26">
         <v>1960</v>
       </c>
-      <c r="V7" s="25" t="s">
+      <c r="V7" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="W7" s="25" t="s">
+      <c r="W7" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="26">
         <v>1980</v>
       </c>
-      <c r="Y7" s="25" t="s">
+      <c r="Y7" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="Z7" s="25" t="s">
+      <c r="Z7" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="AA7" s="25">
+      <c r="AA7" s="26">
         <v>2011</v>
       </c>
-      <c r="AB7" s="25" t="s">
+      <c r="AB7" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="AC7" s="25" t="s">
+      <c r="AC7" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="AD7" s="25">
+      <c r="AD7" s="26">
         <v>2014</v>
       </c>
-      <c r="AE7" s="25" t="s">
+      <c r="AE7" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="AF7" s="25" t="s">
+      <c r="AF7" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="AG7" s="25">
+      <c r="AG7" s="26">
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:44" s="6" customFormat="1" ht="267" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:44" s="7" customFormat="1" ht="267" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:44" s="12" customFormat="1" ht="131" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="S8" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="U8" s="3">
+        <v>1980</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="X8" s="3">
+        <v>1990</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>2002</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" s="13" customFormat="1" ht="131" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="P9" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="Q9" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="R9" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="S9" s="25" t="s">
+      <c r="S9" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="T9" s="25" t="s">
+      <c r="T9" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9" s="26">
         <v>1900</v>
       </c>
-      <c r="V9" s="25" t="s">
+      <c r="V9" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="W9" s="25" t="s">
+      <c r="W9" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="X9" s="25">
+      <c r="X9" s="26">
         <v>1925</v>
       </c>
-      <c r="Y9" s="25" t="s">
+      <c r="Y9" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="Z9" s="25" t="s">
+      <c r="Z9" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="AA9" s="25">
+      <c r="AA9" s="26">
         <v>1975</v>
       </c>
-      <c r="AB9" s="25" t="s">
+      <c r="AB9" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="AC9" s="25" t="s">
+      <c r="AC9" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="AD9" s="25">
+      <c r="AD9" s="26">
         <v>2000</v>
       </c>
-      <c r="AE9" s="25" t="s">
+      <c r="AE9" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="AF9" s="4" t="s">
+      <c r="AF9" s="5" t="s">
         <v>231</v>
+      </c>
+      <c r="AG9" s="13">
+        <v>2016</v>
       </c>
     </row>
     <row r="10" spans="1:44" ht="255" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2370,7 +2449,7 @@
       <c r="F10" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>126</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -2403,60 +2482,60 @@
       <c r="R10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="S10" s="26" t="s">
+      <c r="S10" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="T10" s="27" t="s">
+      <c r="T10" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="U10" s="26">
+      <c r="U10" s="27">
         <v>1970</v>
       </c>
-      <c r="V10" s="26" t="s">
+      <c r="V10" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="W10" s="26" t="s">
+      <c r="W10" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="X10" s="26">
+      <c r="X10" s="27">
         <v>1998</v>
       </c>
-      <c r="Y10" s="26" t="s">
+      <c r="Y10" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="Z10" s="26" t="s">
+      <c r="Z10" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="AA10" s="26">
+      <c r="AA10" s="27">
         <v>2005</v>
       </c>
-      <c r="AB10" s="26" t="s">
+      <c r="AB10" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="AC10" s="26" t="s">
+      <c r="AC10" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="AD10" s="26">
+      <c r="AD10" s="27">
         <v>2015</v>
       </c>
-      <c r="AE10" s="26" t="s">
+      <c r="AE10" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="AF10" s="26" t="s">
+      <c r="AF10" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="AG10" s="26" t="s">
-        <v>206</v>
+      <c r="AG10" s="27">
+        <v>2017</v>
       </c>
     </row>
     <row r="11" spans="1:44" ht="254" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>138</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -2507,11 +2586,11 @@
         <v>322</v>
       </c>
     </row>
-    <row r="13" spans="1:44" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2522,9 +2601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2555,7 +2632,7 @@
       <c r="D2" t="s">
         <v>290</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2569,7 +2646,7 @@
       <c r="D3" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2583,7 +2660,7 @@
       <c r="D4" t="s">
         <v>292</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2597,7 +2674,7 @@
       <c r="D5" t="s">
         <v>293</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2611,7 +2688,7 @@
       <c r="D6" t="s">
         <v>294</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2625,12 +2702,12 @@
       <c r="D7" t="s">
         <v>295</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>259</v>
       </c>
       <c r="C8" t="s">
@@ -2639,12 +2716,12 @@
       <c r="D8" t="s">
         <v>301</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>261</v>
       </c>
       <c r="C9" t="s">
@@ -2653,7 +2730,7 @@
       <c r="D9" t="s">
         <v>297</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2667,7 +2744,7 @@
       <c r="D10" t="s">
         <v>298</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>262</v>
       </c>
     </row>
@@ -2681,7 +2758,7 @@
       <c r="D11" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2695,7 +2772,7 @@
       <c r="D12" t="s">
         <v>300</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="16" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2709,12 +2786,12 @@
       <c r="D13" t="s">
         <v>296</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="20" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>271</v>
       </c>
       <c r="C14" t="s">
@@ -2723,12 +2800,12 @@
       <c r="D14" t="s">
         <v>302</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="17" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>273</v>
       </c>
       <c r="C15" t="s">
@@ -2737,7 +2814,7 @@
       <c r="D15" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="17" t="s">
         <v>272</v>
       </c>
     </row>
@@ -2751,7 +2828,7 @@
       <c r="D16" t="s">
         <v>304</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="17" t="s">
         <v>274</v>
       </c>
     </row>
@@ -2765,7 +2842,7 @@
       <c r="D17" t="s">
         <v>305</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="17" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2779,7 +2856,7 @@
       <c r="D18" t="s">
         <v>306</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="16" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2790,7 +2867,7 @@
       <c r="C19" t="s">
         <v>288</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="16" t="s">
         <v>280</v>
       </c>
     </row>
@@ -2804,7 +2881,7 @@
       <c r="D20" t="s">
         <v>307</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="22" t="s">
         <v>282</v>
       </c>
     </row>
@@ -2815,12 +2892,12 @@
       <c r="C21" t="s">
         <v>288</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>287</v>
       </c>
       <c r="C22" t="s">
@@ -2829,12 +2906,12 @@
       <c r="D22" t="s">
         <v>308</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="23" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="E23" s="22"/>
+      <c r="E23" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>